<commit_message>
updated import interns template
</commit_message>
<xml_diff>
--- a/public/templates/intern_import_template.xlsx
+++ b/public/templates/intern_import_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DIKO\Desktop\Dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{258DECC6-3F94-442F-8148-B94213AEE535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{178A3717-45E3-43C8-BE83-521A0D88788D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{308FEBB1-6E04-4F2C-80AF-E3ADF39918CE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
   <si>
     <t>First Name</t>
   </si>
@@ -65,27 +65,9 @@
     <t>Academic Year</t>
   </si>
   <si>
-    <t>Semeseter</t>
-  </si>
-  <si>
-    <t>Juan</t>
-  </si>
-  <si>
-    <t>Dela Cruz</t>
-  </si>
-  <si>
-    <t>juan.delacruz@evsu.edu.ph</t>
-  </si>
-  <si>
     <t>09123456789</t>
   </si>
   <si>
-    <t>2022-09710</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
     <t>2024-2025</t>
   </si>
   <si>
@@ -98,15 +80,6 @@
     <t>2022-09712</t>
   </si>
   <si>
-    <t>2022-09713</t>
-  </si>
-  <si>
-    <t>2022-09714</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
     <t>Reed</t>
   </si>
   <si>
@@ -119,10 +92,37 @@
     <t>Storm</t>
   </si>
   <si>
-    <t>Bucky</t>
-  </si>
-  <si>
-    <t>Barnes</t>
+    <t>reed.richards@evsu.edu.ph</t>
+  </si>
+  <si>
+    <t>susan.storm@evsu.edu.ph</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>Semester</t>
+  </si>
+  <si>
+    <t>2003-07-09</t>
+  </si>
+  <si>
+    <t>2004-12-23</t>
+  </si>
+  <si>
+    <t>2003-02-14</t>
+  </si>
+  <si>
+    <t>Amadeus</t>
+  </si>
+  <si>
+    <t>Gravoso</t>
+  </si>
+  <si>
+    <t>amadeus.gravoso@evsu.edu.ph</t>
+  </si>
+  <si>
+    <t>2022-09709</t>
   </si>
   <si>
     <t>Peter</t>
@@ -131,25 +131,28 @@
     <t>Parker</t>
   </si>
   <si>
-    <t>reed.richards@evsu.edu.ph</t>
-  </si>
-  <si>
-    <t>susan.storm@evsu.edu.ph</t>
-  </si>
-  <si>
-    <t>bucky.barnes@evsu.edu.ph</t>
-  </si>
-  <si>
     <t>peter.parker@evsu.edu.ph</t>
+  </si>
+  <si>
+    <t>2023-06789</t>
+  </si>
+  <si>
+    <t>2001-08-12</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>male</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="yyyy\-mm\-dd;@"/>
-  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -194,11 +197,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -534,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CA238C1-43A3-43AE-BF1C-73206C78A866}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" zoomScale="162" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -547,14 +549,15 @@
     <col min="3" max="3" width="24.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.81640625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.08984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.90625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.453125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="10.08984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -570,180 +573,160 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
+      <c r="I3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="K3" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="2" t="s">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="3">
-        <v>37890</v>
-      </c>
-      <c r="G2">
+      <c r="F4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4">
         <v>4</v>
       </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" t="s">
-        <v>18</v>
+      <c r="I4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="1" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="3">
-        <v>37814</v>
-      </c>
-      <c r="G3">
+      <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5">
         <v>4</v>
       </c>
-      <c r="H3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="3">
-        <v>37892</v>
-      </c>
-      <c r="G4">
-        <v>4</v>
-      </c>
-      <c r="H4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="I5" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="3">
-        <v>37893</v>
-      </c>
-      <c r="G5">
-        <v>4</v>
-      </c>
-      <c r="H5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" t="s">
-        <v>16</v>
-      </c>
       <c r="J5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="3">
-        <v>37894</v>
-      </c>
-      <c r="G6">
-        <v>4</v>
-      </c>
-      <c r="H6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" t="s">
-        <v>16</v>
-      </c>
-      <c r="J6" t="s">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="K5" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -752,10 +735,9 @@
     <hyperlink ref="C2" r:id="rId1" xr:uid="{20636ABA-993D-4268-997F-185285B71005}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{CC2065AF-1E39-429B-A8FE-272DEEEFAADE}"/>
     <hyperlink ref="C4" r:id="rId3" xr:uid="{0560B419-10EB-4E92-AABE-F369A420920E}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{07C2BA49-8BD5-4B4D-8A95-F95138B73365}"/>
-    <hyperlink ref="C6" r:id="rId5" xr:uid="{3A15DB6D-204A-44F2-BC8A-780483A5FCDE}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{1C69D944-FC15-4376-B8B0-B346F889104C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId6"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>